<commit_message>
Update Gamma Age Mutations Workbook.xlsx
</commit_message>
<xml_diff>
--- a/_notes/Gamma Age Mutations Workbook.xlsx
+++ b/_notes/Gamma Age Mutations Workbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="20115" windowHeight="8265"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="20115" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mutations" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="342">
   <si>
     <t>Mutations that are possible in the NWN / PRC framework</t>
   </si>
@@ -919,6 +919,177 @@
   </si>
   <si>
     <t>Silk Glands</t>
+  </si>
+  <si>
+    <t>Hide -4</t>
+  </si>
+  <si>
+    <t>Search -4 , Spot -4</t>
+  </si>
+  <si>
+    <t>Listen -4, Perform -4</t>
+  </si>
+  <si>
+    <t>Attack -2 &amp; Damage -2 when HP below 25%</t>
+  </si>
+  <si>
+    <t>Fadeout (D)</t>
+  </si>
+  <si>
+    <t>Diminished Hearing (D)</t>
+  </si>
+  <si>
+    <t>Diminished Sight (D)</t>
+  </si>
+  <si>
+    <t>DC 15 Will save or Daze on first round of every combat</t>
+  </si>
+  <si>
+    <t>Will saves -4, can't take Iron Will or Epic Will</t>
+  </si>
+  <si>
+    <t>Mentally Defenseless (D)</t>
+  </si>
+  <si>
+    <t>Noctural (D)</t>
+  </si>
+  <si>
+    <t>Rage (D)</t>
+  </si>
+  <si>
+    <t>Seizures (D)</t>
+  </si>
+  <si>
+    <t>Hide -4, CHA skills -2</t>
+  </si>
+  <si>
+    <t>AC -1</t>
+  </si>
+  <si>
+    <t>Damage vulnerability from all energy sources +10%</t>
+  </si>
+  <si>
+    <t>Stench (D)</t>
+  </si>
+  <si>
+    <t>Thin Hide (D)</t>
+  </si>
+  <si>
+    <t>Energy Sensitivity (D)</t>
+  </si>
+  <si>
+    <t>Amphibious (D)</t>
+  </si>
+  <si>
+    <t>Extreme Metabolism (D)</t>
+  </si>
+  <si>
+    <t>You suffer 50% more damage from bludgeoning &amp; concussion (sonic) damage</t>
+  </si>
+  <si>
+    <t>Brittle Bones (D)</t>
+  </si>
+  <si>
+    <t>33% chance to have an adverse effect from a tonic (potion)  healing tonics still heal HP.</t>
+  </si>
+  <si>
+    <t>Attraction Odor (D)</t>
+  </si>
+  <si>
+    <t>Tonic Allergy (D)</t>
+  </si>
+  <si>
+    <t>DC 12 Fort save on 1st round of Combat or dazed for 1d6 rounds.</t>
+  </si>
+  <si>
+    <t>STR -1</t>
+  </si>
+  <si>
+    <t>Nerve Corruption (D)</t>
+  </si>
+  <si>
+    <t>DEX -1</t>
+  </si>
+  <si>
+    <t>Corpus Corruption (D)</t>
+  </si>
+  <si>
+    <t>Blighted (D)</t>
+  </si>
+  <si>
+    <t>CON -1</t>
+  </si>
+  <si>
+    <t>Low-light Vision but also -3 on all attacks, skills &amp; saves during the day.</t>
+  </si>
+  <si>
+    <t>Needs 4x food.  (Will require integration w/ HCR2), -2 Saves vs poison &amp; disease.</t>
+  </si>
+  <si>
+    <t>Sluggish (D)</t>
+  </si>
+  <si>
+    <t>Sickly (D)</t>
+  </si>
+  <si>
+    <t>Reflex -2, can't take Lightining Reflexes or Epic Reflexes</t>
+  </si>
+  <si>
+    <t>Fortitude  -2, can't take Great Fortitude or Epic Fortitude</t>
+  </si>
+  <si>
+    <t>Bleeder (D)</t>
+  </si>
+  <si>
+    <t>You suffer 25% more damage from piercing &amp; slashing damage</t>
+  </si>
+  <si>
+    <t>Sensitivity to Acid (D)</t>
+  </si>
+  <si>
+    <t>Sensitivity to Cold (D)</t>
+  </si>
+  <si>
+    <t>Sensitivity to Electricity (D)</t>
+  </si>
+  <si>
+    <t>Sensitivity to Fire (D)</t>
+  </si>
+  <si>
+    <t>Sensitivity to Radiation (D)</t>
+  </si>
+  <si>
+    <t>Sensitivity to Concussion (D)</t>
+  </si>
+  <si>
+    <t>You suffer 25% more damage from concussion (sonic)</t>
+  </si>
+  <si>
+    <t>You suffer 25% more damage from acid</t>
+  </si>
+  <si>
+    <t>You suffer 25% more damage from cold</t>
+  </si>
+  <si>
+    <t>You suffer 25% more damage from electricity</t>
+  </si>
+  <si>
+    <t>You suffer 25% more damage from fire</t>
+  </si>
+  <si>
+    <t>You suffer 25% more damage from radiation</t>
+  </si>
+  <si>
+    <t>DC 15 Will save or Shaken in combat</t>
+  </si>
+  <si>
+    <t>DC 20 Will save or Frenzy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain Waterbreathing. Your skin must be kept moist with fresh water. You pour water on yourself rather than drinking it to quench your thirst. You require about two-thirds more water than usual. </t>
+  </si>
+  <si>
+    <t>Heightened Fear Response (D)</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -3880,19 +4051,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34" customWidth="1"/>
+    <col min="5" max="5" width="154.85546875" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="28.42578125" customWidth="1"/>
   </cols>
@@ -3925,29 +4096,30 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>256</v>
+    <row r="4" spans="1:7" s="1" customFormat="1">
+      <c r="A4" s="7" t="s">
+        <v>309</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>257</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E4" t="s">
-        <v>258</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E4" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
@@ -3956,10 +4128,577 @@
         <v>257</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>258</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>290</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>287</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>291</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>286</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>259</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>288</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>292</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>293</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>295</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>318</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>298</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>302</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>299</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>303</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>300</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>304</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>340</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>305</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>319</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>307</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>306</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>315</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>312</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" t="s">
+        <v>308</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>297</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>311</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>313</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>314</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>316</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>317</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>320</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>322</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>321</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>323</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>324</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" t="s">
+        <v>325</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>326</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
+        <v>333</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>327</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>334</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>328</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" t="s">
+        <v>335</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>329</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" t="s">
+        <v>336</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>330</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" t="s">
+        <v>337</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>331</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>332</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>341</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
+        <v>338</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>296</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
+        <v>339</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Started on mutation test scripts
Started on mutation test scripts.
</commit_message>
<xml_diff>
--- a/_notes/Gamma Age Mutations Workbook.xlsx
+++ b/_notes/Gamma Age Mutations Workbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="20115" windowHeight="8265" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="20115" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Mutations" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Minor</t>
-  </si>
-  <si>
-    <t>Climb +8</t>
   </si>
   <si>
     <t>Key Ability Score</t>
@@ -1090,6 +1087,9 @@
   </si>
   <si>
     <t>Heightened Fear Response (D)</t>
+  </si>
+  <si>
+    <t>Climb +8. Grapple + 4</t>
   </si>
 </sst>
 </file>
@@ -1475,11 +1475,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1493,7 +1493,7 @@
     <col min="7" max="7" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1506,42 +1506,42 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1">
       <c r="A4" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>261</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1555,18 +1555,18 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>341</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -1575,38 +1575,38 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -1615,38 +1615,38 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
         <v>197</v>
       </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>198</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -1655,98 +1655,98 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s">
-        <v>33</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>35</v>
       </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -1755,665 +1755,665 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
         <v>45</v>
       </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" t="s">
-        <v>46</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
         <v>48</v>
       </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" t="s">
-        <v>49</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
         <v>50</v>
       </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>51</v>
       </c>
-      <c r="E21" t="s">
-        <v>52</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
         <v>53</v>
       </c>
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" t="s">
-        <v>54</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
         <v>55</v>
       </c>
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" t="s">
-        <v>56</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
         <v>57</v>
       </c>
-      <c r="B24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" t="s">
-        <v>58</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" t="s">
         <v>59</v>
       </c>
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" t="s">
-        <v>60</v>
-      </c>
       <c r="F25" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
         <v>61</v>
       </c>
-      <c r="B26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" t="s">
-        <v>62</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
         <v>184</v>
       </c>
-      <c r="B29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" t="s">
-        <v>185</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
         <v>64</v>
       </c>
-      <c r="B30" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" t="s">
-        <v>65</v>
-      </c>
       <c r="F30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
         <v>68</v>
       </c>
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" t="s">
-        <v>69</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
         <v>70</v>
       </c>
-      <c r="B32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" t="s">
-        <v>71</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
         <v>72</v>
       </c>
-      <c r="B34" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" t="s">
-        <v>73</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
         <v>66</v>
       </c>
-      <c r="B35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" t="s">
-        <v>67</v>
-      </c>
       <c r="F35" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" t="s">
         <v>84</v>
       </c>
-      <c r="B43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" t="s">
-        <v>35</v>
-      </c>
-      <c r="E43" t="s">
-        <v>85</v>
-      </c>
       <c r="F43" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E44" t="s">
+        <v>87</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s">
         <v>90</v>
       </c>
-      <c r="B45" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" t="s">
-        <v>91</v>
-      </c>
       <c r="F45" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" t="s">
         <v>92</v>
       </c>
-      <c r="B46" t="s">
-        <v>27</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" t="s">
-        <v>16</v>
-      </c>
-      <c r="E46" t="s">
-        <v>93</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
         <v>4</v>
@@ -2422,319 +2422,319 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" t="s">
         <v>98</v>
       </c>
-      <c r="B49" t="s">
-        <v>27</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" t="s">
-        <v>16</v>
-      </c>
-      <c r="E49" t="s">
-        <v>99</v>
-      </c>
       <c r="F49" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" t="s">
         <v>101</v>
       </c>
-      <c r="B57" t="s">
-        <v>31</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" t="s">
-        <v>16</v>
-      </c>
-      <c r="E57" t="s">
-        <v>102</v>
-      </c>
       <c r="F57" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B59" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E60" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B61" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E61" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E62" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B63" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
         <v>4</v>
@@ -2743,118 +2743,118 @@
         <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B65" t="s">
         <v>4</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E65" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B66" t="s">
         <v>4</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D66" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E66" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B67" t="s">
         <v>4</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E67" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B68" t="s">
         <v>4</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D68" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E68" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B69" t="s">
         <v>4</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D69" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E69" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B70" t="s">
         <v>4</v>
@@ -2863,38 +2863,38 @@
         <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E70" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B71" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E71" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B72" t="s">
         <v>4</v>
@@ -2903,38 +2903,38 @@
         <v>5</v>
       </c>
       <c r="D72" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E72" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
+        <v>139</v>
+      </c>
+      <c r="B73" t="s">
+        <v>31</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" t="s">
         <v>140</v>
       </c>
-      <c r="B73" t="s">
-        <v>32</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73" t="s">
-        <v>35</v>
-      </c>
-      <c r="E73" t="s">
-        <v>141</v>
-      </c>
       <c r="F73" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B74" t="s">
         <v>4</v>
@@ -2943,318 +2943,318 @@
         <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E74" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
+        <v>137</v>
+      </c>
+      <c r="B75" t="s">
+        <v>31</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" t="s">
+        <v>34</v>
+      </c>
+      <c r="E75" t="s">
         <v>138</v>
       </c>
-      <c r="B75" t="s">
-        <v>32</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D75" t="s">
-        <v>35</v>
-      </c>
-      <c r="E75" t="s">
-        <v>139</v>
-      </c>
       <c r="F75" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B76" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E76" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B77" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E77" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B78" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E78" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B79" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E79" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B80" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E80" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B81" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E81" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B82" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E82" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B83" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E83" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B84" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E84" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B85" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E85" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B86" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E86" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B87" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E87" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
+        <v>164</v>
+      </c>
+      <c r="B88" t="s">
+        <v>26</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D88" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" t="s">
         <v>165</v>
       </c>
-      <c r="B88" t="s">
-        <v>27</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D88" t="s">
-        <v>10</v>
-      </c>
-      <c r="E88" t="s">
-        <v>166</v>
-      </c>
       <c r="F88" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
+        <v>166</v>
+      </c>
+      <c r="B89" t="s">
+        <v>26</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" t="s">
+        <v>15</v>
+      </c>
+      <c r="E89" t="s">
         <v>167</v>
       </c>
-      <c r="B89" t="s">
-        <v>27</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D89" t="s">
-        <v>16</v>
-      </c>
-      <c r="E89" t="s">
-        <v>168</v>
-      </c>
       <c r="F89" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B90" t="s">
         <v>4</v>
@@ -3263,81 +3263,81 @@
         <v>5</v>
       </c>
       <c r="D90" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E90" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
+        <v>185</v>
+      </c>
+      <c r="B91" t="s">
+        <v>31</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" t="s">
+        <v>15</v>
+      </c>
+      <c r="E91" t="s">
         <v>186</v>
       </c>
-      <c r="B91" t="s">
-        <v>32</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D91" t="s">
-        <v>16</v>
-      </c>
-      <c r="E91" t="s">
-        <v>187</v>
-      </c>
       <c r="F91" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
+        <v>170</v>
+      </c>
+      <c r="B92" t="s">
+        <v>26</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D92" t="s">
+        <v>15</v>
+      </c>
+      <c r="E92" t="s">
         <v>171</v>
       </c>
-      <c r="B92" t="s">
-        <v>27</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D92" t="s">
-        <v>16</v>
-      </c>
-      <c r="E92" t="s">
+      <c r="F92" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G92" t="s">
         <v>172</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G92" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
+        <v>248</v>
+      </c>
+      <c r="B93" t="s">
+        <v>31</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>15</v>
+      </c>
+      <c r="E93" t="s">
         <v>249</v>
       </c>
-      <c r="B93" t="s">
-        <v>32</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D93" t="s">
-        <v>16</v>
-      </c>
-      <c r="E93" t="s">
-        <v>250</v>
-      </c>
       <c r="F93" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B94" t="s">
         <v>4</v>
@@ -3346,118 +3346,118 @@
         <v>5</v>
       </c>
       <c r="D94" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E94" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
+        <v>174</v>
+      </c>
+      <c r="B95" t="s">
+        <v>26</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D95" t="s">
+        <v>15</v>
+      </c>
+      <c r="E95" t="s">
         <v>175</v>
       </c>
-      <c r="B95" t="s">
-        <v>27</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D95" t="s">
-        <v>16</v>
-      </c>
-      <c r="E95" t="s">
-        <v>176</v>
-      </c>
       <c r="F95" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
+        <v>176</v>
+      </c>
+      <c r="B96" t="s">
+        <v>26</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D96" t="s">
+        <v>15</v>
+      </c>
+      <c r="E96" t="s">
         <v>177</v>
       </c>
-      <c r="B96" t="s">
-        <v>27</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D96" t="s">
-        <v>16</v>
-      </c>
-      <c r="E96" t="s">
-        <v>178</v>
-      </c>
       <c r="F96" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
+        <v>178</v>
+      </c>
+      <c r="B97" t="s">
+        <v>26</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D97" t="s">
+        <v>15</v>
+      </c>
+      <c r="E97" t="s">
         <v>179</v>
       </c>
-      <c r="B97" t="s">
-        <v>27</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D97" t="s">
-        <v>16</v>
-      </c>
-      <c r="E97" t="s">
-        <v>180</v>
-      </c>
       <c r="F97" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B98" t="s">
         <v>4</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D98" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E98" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
+        <v>181</v>
+      </c>
+      <c r="B99" t="s">
+        <v>26</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D99" t="s">
+        <v>15</v>
+      </c>
+      <c r="E99" t="s">
         <v>182</v>
       </c>
-      <c r="B99" t="s">
-        <v>27</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D99" t="s">
-        <v>16</v>
-      </c>
-      <c r="E99" t="s">
-        <v>183</v>
-      </c>
       <c r="F99" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B100" t="s">
         <v>4</v>
@@ -3466,167 +3466,167 @@
         <v>5</v>
       </c>
       <c r="D100" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E100" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B101" t="s">
         <v>4</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D101" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E101" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="15" customHeight="1">
       <c r="A102" t="s">
+        <v>191</v>
+      </c>
+      <c r="B102" t="s">
+        <v>31</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" t="s">
+        <v>15</v>
+      </c>
+      <c r="E102" t="s">
         <v>192</v>
       </c>
-      <c r="B102" t="s">
-        <v>32</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D102" t="s">
-        <v>16</v>
-      </c>
-      <c r="E102" t="s">
+      <c r="F102" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G102" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G102" s="4" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B103" t="s">
         <v>4</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D103" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E103" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" customHeight="1">
       <c r="A104" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B104" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D104" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E104" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="15" customHeight="1">
       <c r="A105" t="s">
+        <v>199</v>
+      </c>
+      <c r="B105" t="s">
+        <v>30</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D105" t="s">
+        <v>34</v>
+      </c>
+      <c r="E105" t="s">
         <v>200</v>
       </c>
-      <c r="B105" t="s">
-        <v>31</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D105" t="s">
-        <v>35</v>
-      </c>
-      <c r="E105" t="s">
-        <v>201</v>
-      </c>
       <c r="F105" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
+        <v>201</v>
+      </c>
+      <c r="B106" t="s">
+        <v>26</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" t="s">
+        <v>15</v>
+      </c>
+      <c r="E106" t="s">
         <v>202</v>
       </c>
-      <c r="B106" t="s">
-        <v>27</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D106" t="s">
-        <v>16</v>
-      </c>
-      <c r="E106" t="s">
-        <v>203</v>
-      </c>
       <c r="F106" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B107" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D107" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E107" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B108" t="s">
         <v>4</v>
@@ -3635,161 +3635,161 @@
         <v>5</v>
       </c>
       <c r="D108" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E108" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B109" t="s">
         <v>4</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D109" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E109" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" t="s">
+        <v>30</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110" t="s">
         <v>219</v>
       </c>
-      <c r="B110" t="s">
-        <v>31</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D110" t="s">
-        <v>10</v>
-      </c>
-      <c r="E110" t="s">
-        <v>220</v>
-      </c>
       <c r="F110" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
+        <v>215</v>
+      </c>
+      <c r="B111" t="s">
+        <v>26</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" t="s">
+        <v>15</v>
+      </c>
+      <c r="E111" t="s">
         <v>216</v>
       </c>
-      <c r="B111" t="s">
-        <v>27</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D111" t="s">
-        <v>16</v>
-      </c>
-      <c r="E111" t="s">
+      <c r="F111" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G111" t="s">
         <v>217</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G111" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
+        <v>221</v>
+      </c>
+      <c r="B112" t="s">
+        <v>31</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D112" t="s">
+        <v>15</v>
+      </c>
+      <c r="E112" t="s">
         <v>222</v>
       </c>
-      <c r="B112" t="s">
-        <v>32</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D112" t="s">
-        <v>16</v>
-      </c>
-      <c r="E112" t="s">
-        <v>223</v>
-      </c>
       <c r="F112" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B113" t="s">
         <v>4</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D113" t="s">
+        <v>23</v>
+      </c>
+      <c r="E113" t="s">
         <v>24</v>
       </c>
-      <c r="E113" t="s">
-        <v>25</v>
-      </c>
       <c r="F113" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
+        <v>223</v>
+      </c>
+      <c r="B114" t="s">
+        <v>31</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D114" t="s">
+        <v>210</v>
+      </c>
+      <c r="E114" t="s">
         <v>224</v>
       </c>
-      <c r="B114" t="s">
-        <v>32</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D114" t="s">
-        <v>211</v>
-      </c>
-      <c r="E114" t="s">
-        <v>225</v>
-      </c>
       <c r="F114" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B115" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D115" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E115" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B116" t="s">
         <v>4</v>
@@ -3798,18 +3798,18 @@
         <v>5</v>
       </c>
       <c r="D116" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E116" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B117" t="s">
         <v>4</v>
@@ -3818,58 +3818,58 @@
         <v>5</v>
       </c>
       <c r="D117" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E117" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B118" t="s">
         <v>4</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D118" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E118" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B119" t="s">
         <v>4</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D119" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E119" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B120" t="s">
         <v>4</v>
@@ -3878,173 +3878,173 @@
         <v>5</v>
       </c>
       <c r="D120" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E120" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
+        <v>236</v>
+      </c>
+      <c r="B121" t="s">
+        <v>26</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D121" t="s">
+        <v>15</v>
+      </c>
+      <c r="E121" t="s">
         <v>237</v>
       </c>
-      <c r="B121" t="s">
-        <v>27</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D121" t="s">
-        <v>16</v>
-      </c>
-      <c r="E121" t="s">
-        <v>238</v>
-      </c>
       <c r="F121" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
+        <v>238</v>
+      </c>
+      <c r="B122" t="s">
+        <v>26</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D122" t="s">
+        <v>15</v>
+      </c>
+      <c r="E122" t="s">
         <v>239</v>
       </c>
-      <c r="B122" t="s">
-        <v>27</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D122" t="s">
-        <v>16</v>
-      </c>
-      <c r="E122" t="s">
-        <v>240</v>
-      </c>
       <c r="F122" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
+        <v>240</v>
+      </c>
+      <c r="B123" t="s">
+        <v>26</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D123" t="s">
+        <v>15</v>
+      </c>
+      <c r="E123" t="s">
         <v>241</v>
       </c>
-      <c r="B123" t="s">
-        <v>27</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D123" t="s">
-        <v>16</v>
-      </c>
-      <c r="E123" t="s">
-        <v>242</v>
-      </c>
       <c r="F123" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
+        <v>242</v>
+      </c>
+      <c r="B124" t="s">
+        <v>26</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D124" t="s">
+        <v>15</v>
+      </c>
+      <c r="E124" t="s">
         <v>243</v>
       </c>
-      <c r="B124" t="s">
-        <v>27</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D124" t="s">
-        <v>16</v>
-      </c>
-      <c r="E124" t="s">
-        <v>244</v>
-      </c>
       <c r="F124" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B125" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D125" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E125" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
+        <v>244</v>
+      </c>
+      <c r="B126" t="s">
+        <v>30</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D126" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" t="s">
         <v>245</v>
       </c>
-      <c r="B126" t="s">
-        <v>31</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D126" t="s">
-        <v>10</v>
-      </c>
-      <c r="E126" t="s">
-        <v>246</v>
-      </c>
       <c r="F126" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
+        <v>246</v>
+      </c>
+      <c r="B127" t="s">
+        <v>31</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D127" t="s">
+        <v>9</v>
+      </c>
+      <c r="E127" t="s">
         <v>247</v>
       </c>
-      <c r="B127" t="s">
-        <v>32</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D127" t="s">
-        <v>10</v>
-      </c>
-      <c r="E127" t="s">
-        <v>248</v>
-      </c>
       <c r="F127" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B128" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D128" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E128" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -4062,8 +4062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4079,7 +4079,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1">
@@ -4090,620 +4090,620 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1">
       <c r="A4" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
         <v>257</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" t="s">
-        <v>258</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
+        <v>312</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
         <v>313</v>
       </c>
-      <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" t="s">
-        <v>314</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
+        <v>315</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" t="s">
         <v>316</v>
       </c>
-      <c r="B22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" t="s">
-        <v>317</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
+        <v>323</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" t="s">
         <v>324</v>
       </c>
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" t="s">
-        <v>325</v>
-      </c>
       <c r="F25" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
+        <v>330</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" t="s">
         <v>331</v>
       </c>
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" t="s">
-        <v>332</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More mutation test scripts
More mutation test scripts.
</commit_message>
<xml_diff>
--- a/_notes/Gamma Age Mutations Workbook.xlsx
+++ b/_notes/Gamma Age Mutations Workbook.xlsx
@@ -1476,10 +1476,10 @@
   <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Mutation test scripts wrap-up
Mutation test scripts wrap-up.  First batch of mutation test scripts is complete.
</commit_message>
<xml_diff>
--- a/_notes/Gamma Age Mutations Workbook.xlsx
+++ b/_notes/Gamma Age Mutations Workbook.xlsx
@@ -706,15 +706,6 @@
     <t>As Metamrophosis but ranged, 20 + WIS Bonus * 5 minutes &amp; can only use every 3 hours.</t>
   </si>
   <si>
-    <t>Size Change, Large</t>
-  </si>
-  <si>
-    <t>Increase size -1 AC, -1 Attack, -4 Stealth. (7’ - 13’ high.), Attributes &amp; speed don't change</t>
-  </si>
-  <si>
-    <t>Size Change, Small</t>
-  </si>
-  <si>
     <t>Skeletal Enhancement</t>
   </si>
   <si>
@@ -740,9 +731,6 @@
   </si>
   <si>
     <t>2d6 + STR Bonus concussion damage in a 20' + STR Bonus range cone, usable 3 + CON Bonus / day, Deafen DC = 10 + 1/2 HD + STR Bonus</t>
-  </si>
-  <si>
-    <t>Decrease Size, +1 AC, +1 Attack, +4 Stealth. (Less than 4’ 6” high.), Attributes &amp; speed don't change</t>
   </si>
   <si>
     <t>Stunning Force</t>
@@ -1090,6 +1078,18 @@
   </si>
   <si>
     <t>Tremorsense, +3 craft skills</t>
+  </si>
+  <si>
+    <t>Increase size -1 AC, -1 Attack, -4 Stealth. (7’ - 13’ high.), speed doesn't change</t>
+  </si>
+  <si>
+    <t>Decrease Size, +1 AC, +1 Attack, +4 Stealth. (Less than 4’ 6” high.), speed doesn't change</t>
+  </si>
+  <si>
+    <t>Size Change, Larger</t>
+  </si>
+  <si>
+    <t>Size Change, Smaller</t>
   </si>
 </sst>
 </file>
@@ -1476,10 +1476,10 @@
   <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B115" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E76" sqref="E76"/>
+      <selection pane="bottomRight" activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1">
       <c r="A4" s="7" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>30</v>
@@ -1535,13 +1535,13 @@
         <v>15</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1558,7 +1558,7 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -1999,7 +1999,7 @@
         <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>42</v>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B37" t="s">
         <v>31</v>
@@ -2207,7 +2207,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B38" t="s">
         <v>31</v>
@@ -2227,7 +2227,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B39" t="s">
         <v>31</v>
@@ -2247,7 +2247,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B40" t="s">
         <v>31</v>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B41" t="s">
         <v>31</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B42" t="s">
         <v>31</v>
@@ -2425,7 +2425,7 @@
         <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>7</v>
@@ -2754,7 +2754,7 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B65" t="s">
         <v>4</v>
@@ -2766,7 +2766,7 @@
         <v>50</v>
       </c>
       <c r="E65" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>22</v>
@@ -2774,7 +2774,7 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B66" t="s">
         <v>4</v>
@@ -2786,7 +2786,7 @@
         <v>50</v>
       </c>
       <c r="E66" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>22</v>
@@ -2794,7 +2794,7 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B67" t="s">
         <v>4</v>
@@ -2806,7 +2806,7 @@
         <v>50</v>
       </c>
       <c r="E67" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>22</v>
@@ -2814,7 +2814,7 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B68" t="s">
         <v>31</v>
@@ -2826,7 +2826,7 @@
         <v>50</v>
       </c>
       <c r="E68" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>42</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B69" t="s">
         <v>4</v>
@@ -2846,7 +2846,7 @@
         <v>50</v>
       </c>
       <c r="E69" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>22</v>
@@ -2966,7 +2966,7 @@
         <v>34</v>
       </c>
       <c r="E75" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>7</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B77" t="s">
         <v>31</v>
@@ -3317,7 +3317,7 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B93" t="s">
         <v>31</v>
@@ -3329,7 +3329,7 @@
         <v>15</v>
       </c>
       <c r="E93" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>22</v>
@@ -3558,7 +3558,7 @@
         <v>22</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="15" customHeight="1">
@@ -3729,7 +3729,7 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B113" t="s">
         <v>4</v>
@@ -3749,19 +3749,19 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>221</v>
+        <v>340</v>
       </c>
       <c r="B114" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D114" t="s">
-        <v>208</v>
+        <v>15</v>
       </c>
       <c r="E114" t="s">
-        <v>222</v>
+        <v>338</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>7</v>
@@ -3769,19 +3769,19 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>223</v>
+        <v>341</v>
       </c>
       <c r="B115" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D115" t="s">
-        <v>208</v>
+        <v>15</v>
       </c>
       <c r="E115" t="s">
-        <v>233</v>
+        <v>339</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>7</v>
@@ -3789,7 +3789,7 @@
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B116" t="s">
         <v>4</v>
@@ -3801,7 +3801,7 @@
         <v>208</v>
       </c>
       <c r="E116" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>7</v>
@@ -3809,7 +3809,7 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B117" t="s">
         <v>4</v>
@@ -3821,7 +3821,7 @@
         <v>15</v>
       </c>
       <c r="E117" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>22</v>
@@ -3829,7 +3829,7 @@
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B118" t="s">
         <v>4</v>
@@ -3841,15 +3841,15 @@
         <v>15</v>
       </c>
       <c r="E118" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B119" t="s">
         <v>4</v>
@@ -3861,10 +3861,10 @@
         <v>15</v>
       </c>
       <c r="E119" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3889,7 +3889,7 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B121" t="s">
         <v>26</v>
@@ -3901,7 +3901,7 @@
         <v>15</v>
       </c>
       <c r="E121" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>42</v>
@@ -3909,7 +3909,7 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B122" t="s">
         <v>26</v>
@@ -3921,7 +3921,7 @@
         <v>15</v>
       </c>
       <c r="E122" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>42</v>
@@ -3929,7 +3929,7 @@
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B123" t="s">
         <v>26</v>
@@ -3941,7 +3941,7 @@
         <v>15</v>
       </c>
       <c r="E123" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>42</v>
@@ -3949,7 +3949,7 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B124" t="s">
         <v>26</v>
@@ -3961,7 +3961,7 @@
         <v>15</v>
       </c>
       <c r="E124" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>42</v>
@@ -3969,7 +3969,7 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B125" t="s">
         <v>26</v>
@@ -3981,7 +3981,7 @@
         <v>15</v>
       </c>
       <c r="E125" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>42</v>
@@ -3989,7 +3989,7 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B126" t="s">
         <v>30</v>
@@ -4001,7 +4001,7 @@
         <v>9</v>
       </c>
       <c r="E126" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>7</v>
@@ -4009,7 +4009,7 @@
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B127" t="s">
         <v>31</v>
@@ -4021,7 +4021,7 @@
         <v>9</v>
       </c>
       <c r="E127" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>22</v>
@@ -4029,7 +4029,7 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B128" t="s">
         <v>26</v>
@@ -4041,7 +4041,7 @@
         <v>15</v>
       </c>
       <c r="E128" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>42</v>
@@ -4079,7 +4079,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1">
@@ -4107,19 +4107,19 @@
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1">
       <c r="A4" s="7" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>7</v>
@@ -4128,19 +4128,19 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
@@ -4148,19 +4148,19 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>7</v>
@@ -4168,19 +4168,19 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>7</v>
@@ -4188,19 +4188,19 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>7</v>
@@ -4208,19 +4208,19 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>7</v>
@@ -4228,19 +4228,19 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>7</v>
@@ -4248,19 +4248,19 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>7</v>
@@ -4268,19 +4268,19 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>7</v>
@@ -4288,19 +4288,19 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>7</v>
@@ -4308,19 +4308,19 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>7</v>
@@ -4328,19 +4328,19 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B15" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>7</v>
@@ -4348,19 +4348,19 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>7</v>
@@ -4368,19 +4368,19 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>7</v>
@@ -4388,19 +4388,19 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>7</v>
@@ -4408,19 +4408,19 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>7</v>
@@ -4428,19 +4428,19 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>7</v>
@@ -4448,19 +4448,19 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B21" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>7</v>
@@ -4468,19 +4468,19 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B22" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>7</v>
@@ -4488,19 +4488,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>7</v>
@@ -4508,19 +4508,19 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B24" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>7</v>
@@ -4528,19 +4528,19 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B25" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>7</v>
@@ -4548,19 +4548,19 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B26" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>7</v>
@@ -4568,19 +4568,19 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B27" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>7</v>
@@ -4588,19 +4588,19 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>7</v>
@@ -4608,19 +4608,19 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>7</v>
@@ -4628,19 +4628,19 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>7</v>
@@ -4648,19 +4648,19 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E31" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>7</v>
@@ -4668,19 +4668,19 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B32" t="s">
         <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>7</v>
@@ -4688,19 +4688,19 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="9" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B33" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Started mutation maintenance scripts
Started mutation maintenance scripts.
</commit_message>
<xml_diff>
--- a/_notes/Gamma Age Mutations Workbook.xlsx
+++ b/_notes/Gamma Age Mutations Workbook.xlsx
@@ -1127,12 +1127,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1156,7 +1162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1179,6 +1185,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1476,10 +1486,10 @@
   <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B115" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E128" sqref="E128"/>
+      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1544,43 +1554,43 @@
         <v>255</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" s="10" customFormat="1">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+      <c r="F5" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="10" customFormat="1">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1724,23 +1734,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
+    <row r="14" spans="1:7" s="10" customFormat="1">
+      <c r="A14" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="B14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1825,23 +1835,23 @@
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
+    <row r="19" spans="1:7" s="10" customFormat="1">
+      <c r="A19" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="B19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1965,23 +1975,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
+    <row r="26" spans="1:7" s="10" customFormat="1">
+      <c r="A26" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="B26" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="11" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>